<commit_message>
Validate an Blank lines
</commit_message>
<xml_diff>
--- a/Original Sheets/Edited.xlsx
+++ b/Original Sheets/Edited.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juancarlosjr97/Documents/GitHub/Layer9DragDropValidation/Original Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE99D42-B690-F244-B1F3-EED7D11C9004}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C470E3-FEE3-B14D-BC5B-816464760D21}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="1500" windowWidth="25040" windowHeight="14500" xr2:uid="{4A2C9FF7-1BE1-DD48-BB33-CDF74B9795B8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7791" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7804" uniqueCount="70">
   <si>
     <t>invoicenumber</t>
   </si>
@@ -220,6 +220,21 @@
   </si>
   <si>
     <t>SE218EN</t>
+  </si>
+  <si>
+    <t>Layer 10</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>771 L Bin</t>
+  </si>
+  <si>
+    <t>19 01 04</t>
+  </si>
+  <si>
+    <t>D2</t>
   </si>
 </sst>
 </file>
@@ -599,11 +614,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1979303-7BB9-094C-A226-60BA4BA24039}">
-  <dimension ref="A1:U556"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{521B9C2E-11BD-754D-B2EC-563AB7EF5A8C}">
+  <dimension ref="A1:U557"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="D545" workbookViewId="0">
+      <selection activeCell="R560" sqref="R560"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -36748,6 +36763,69 @@
         <v>15.65</v>
       </c>
     </row>
+    <row r="557" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A557" s="6"/>
+      <c r="B557" s="7">
+        <v>43372</v>
+      </c>
+      <c r="C557">
+        <v>201809</v>
+      </c>
+      <c r="D557">
+        <v>9002457</v>
+      </c>
+      <c r="E557" t="s">
+        <v>65</v>
+      </c>
+      <c r="F557" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G557" t="s">
+        <v>61</v>
+      </c>
+      <c r="H557" t="s">
+        <v>62</v>
+      </c>
+      <c r="I557" t="s">
+        <v>23</v>
+      </c>
+      <c r="J557" t="s">
+        <v>63</v>
+      </c>
+      <c r="K557" t="s">
+        <v>64</v>
+      </c>
+      <c r="L557" t="s">
+        <v>27</v>
+      </c>
+      <c r="M557" t="s">
+        <v>67</v>
+      </c>
+      <c r="N557" t="s">
+        <v>29</v>
+      </c>
+      <c r="O557" t="s">
+        <v>68</v>
+      </c>
+      <c r="P557" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q557" t="s">
+        <v>32</v>
+      </c>
+      <c r="R557">
+        <v>1</v>
+      </c>
+      <c r="S557" s="8">
+        <v>60</v>
+      </c>
+      <c r="T557" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="U557" s="10">
+        <v>16.649999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>